<commit_message>
Oil Pricing and max visualization
</commit_message>
<xml_diff>
--- a/data/Oil Pricing.xlsx
+++ b/data/Oil Pricing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maximogonzalez/Documents/GitHub/Blog-Internet_Explorers/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F467D72-A8EC-674F-8FB0-7B60888E6C6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A49CFC29-D4F0-C849-9116-728EA758D112}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{B2205308-9D2D-2542-9D65-840E6FDFB2E6}"/>
   </bookViews>
@@ -38,19 +38,19 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
-    <t>Date</t>
+    <t>date</t>
   </si>
   <si>
-    <t>Month</t>
+    <t>US_pricing</t>
   </si>
   <si>
-    <t>Year</t>
+    <t>month</t>
   </si>
   <si>
-    <t>US_Pricing</t>
+    <t>year</t>
   </si>
   <si>
-    <t>Europe_Pricing</t>
+    <t>europe_pricing</t>
   </si>
 </sst>
 </file>
@@ -440,16 +440,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>